<commit_message>
Can read an excel order, and handle the order as single pallets or combo pallets!
</commit_message>
<xml_diff>
--- a/client-only/Coop.xlsx
+++ b/client-only/Coop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samis-mac/My Drive/Courses/Fullstack-Development/Palletize-JS/client-only/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A92D48-C554-8F4A-93EA-061EC0C50A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9357708A-0E21-0740-BC0B-618932FB69A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33240" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{176E6E39-73AA-8C43-80B7-FB166E0FB9CC}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +578,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>120</v>
+        <v>1266</v>
       </c>
       <c r="B14" s="3">
         <v>20</v>

</xml_diff>